<commit_message>
Módulo 05 - Formulas: Datas
</commit_message>
<xml_diff>
--- a/módulo 05/aula-formulas-data-hora.xlsx
+++ b/módulo 05/aula-formulas-data-hora.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\05 Primeiras fórmulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -157,6 +157,12 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>Funções : data atual --&gt; =Hoje() - agora()</t>
+  </si>
+  <si>
+    <t>Para formatar datas com contas de dias a célula deve ser do tipo geral ou número</t>
+  </si>
 </sst>
 </file>
 
@@ -239,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -301,11 +307,55 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -322,14 +372,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>502875</xdr:rowOff>
     </xdr:to>
@@ -339,7 +389,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -412,6 +462,531 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>887010</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>473056</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CaixaDeTexto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28575" y="28575"/>
+          <a:ext cx="1687110" cy="444481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="72000" rIns="72000" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>Educandoweb</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="100">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Gestão</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> de Frotas</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>261937</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>502875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Retângulo: Cantos Superiores Recortados 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3462337" y="142875"/>
+          <a:ext cx="1438275" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000" b="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Cadastros</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>502875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4924424" y="142875"/>
+          <a:ext cx="1438275" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000" b="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Manutenção</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>90486</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>700086</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>502875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6386511" y="142875"/>
+          <a:ext cx="1438275" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="pt-BR" sz="1000" b="0">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>502875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848600" y="142875"/>
+          <a:ext cx="1438275" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="pt-BR" sz="1000" b="0">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>502875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo: Cantos Superiores Recortados 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2000250" y="142875"/>
+          <a:ext cx="1438275" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000" b="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Início</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>58335</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -422,7 +997,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -542,7 +1117,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -560,7 +1135,9 @@
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent3"/>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="90000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -586,7 +1163,7 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
             <a:rPr lang="pt-BR" sz="1000" b="0">
               <a:solidFill>
@@ -623,7 +1200,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -704,7 +1281,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -782,534 +1359,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7848600" y="142875"/>
-          <a:ext cx="1438275" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="snip2SameRect">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="pt-BR" sz="1000" b="0">
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>502875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Retângulo: Cantos Superiores Recortados 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2000250" y="142875"/>
-          <a:ext cx="1438275" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="snip2SameRect">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1000" b="0">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Início</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>58335</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>473056</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CaixaDeTexto 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="28575" y="28575"/>
-          <a:ext cx="1687110" cy="444481"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="72000" rIns="72000" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1800">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
-              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
-            </a:rPr>
-            <a:t>Educandoweb</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="pt-BR" sz="100">
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1000">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Gestão</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1000" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> de Frotas</a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1000">
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="95000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>757237</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>502875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo: Cantos Superiores Recortados 3">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3462337" y="142875"/>
-          <a:ext cx="1438275" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="snip2SameRect">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="90000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1000" b="0">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Cadastros</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>781049</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>502875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4924424" y="142875"/>
-          <a:ext cx="1438275" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="snip2SameRect">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1000" b="0">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Manutenção</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>585786</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>366711</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>502875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6386511" y="142875"/>
-          <a:ext cx="1438275" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="snip2SameRect">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="54000" rIns="54000" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="pt-BR" sz="1000" b="0">
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>502875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1388,7 +1438,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1470,7 +1520,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1558,7 +1608,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1651,7 +1701,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1732,7 +1782,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1852,7 +1902,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1935,7 +1985,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2016,7 +2066,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2094,7 +2144,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2173,7 +2223,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2261,7 +2311,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2343,7 +2393,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2436,7 +2486,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2517,7 +2567,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2637,7 +2687,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2720,7 +2770,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2801,7 +2851,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2879,7 +2929,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2958,7 +3008,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3046,7 +3096,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3134,7 +3184,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3499,13 +3549,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="12.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
+    <col min="3" max="15" width="12.42578125" style="1" customWidth="1"/>
     <col min="16" max="16" width="2.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="11.7109375" style="1" hidden="1"/>
   </cols>
@@ -3577,12 +3629,34 @@
         <v>Rua Do Educador, 2500 - Uberlândia</v>
       </c>
     </row>
-    <row r="24" spans="13:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="25">
+        <f ca="1">TODAY()</f>
+        <v>45348</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="26">
+        <f ca="1">NOW()</f>
+        <v>45348.726684259258</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M24" s="23"/>
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
     </row>
-    <row r="25" spans="13:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
@@ -4474,8 +4548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4484,7 +4558,8 @@
     <col min="2" max="3" width="32.42578125" style="1" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
-    <col min="7" max="10" width="12.42578125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="3.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="2.42578125" style="1" customWidth="1"/>
     <col min="16" max="16" width="2.28515625" style="1" hidden="1" customWidth="1"/>
@@ -4550,6 +4625,9 @@
       <c r="H4" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="J4" s="25">
+        <v>45005</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
@@ -4571,9 +4649,12 @@
         <v>34</v>
       </c>
       <c r="G5" s="15">
-        <v>45202</v>
-      </c>
-      <c r="H5" s="17"/>
+        <v>45933</v>
+      </c>
+      <c r="H5" s="17">
+        <f ca="1">G5-TODAY()</f>
+        <v>585</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -4602,9 +4683,12 @@
         <v>38</v>
       </c>
       <c r="G6" s="15">
-        <v>45560</v>
-      </c>
-      <c r="H6" s="17"/>
+        <v>45285</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" ref="H6:H7" ca="1" si="0">G6-TODAY()</f>
+        <v>-63</v>
+      </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -4631,11 +4715,17 @@
         <v>42</v>
       </c>
       <c r="G7" s="15">
-        <v>45265</v>
-      </c>
-      <c r="H7" s="17"/>
+        <v>45631</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>283</v>
+      </c>
       <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="J7" s="27">
+        <f ca="1">J4-TODAY()</f>
+        <v>-343</v>
+      </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
@@ -5362,6 +5452,14 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
+  <conditionalFormatting sqref="H5:H7">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Categoria Inválida!" error="Selecione uma das categorias disponíveis." sqref="F5:F18">
       <formula1>"A,B,C,D,E,AB,AC,AD,AE"</formula1>

</xml_diff>

<commit_message>
Módulo 05 - Formulas: Datas finalização
</commit_message>
<xml_diff>
--- a/módulo 05/aula-formulas-data-hora.xlsx
+++ b/módulo 05/aula-formulas-data-hora.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -162,6 +162,24 @@
   </si>
   <si>
     <t>Para formatar datas com contas de dias a célula deve ser do tipo geral ou número</t>
+  </si>
+  <si>
+    <t>Extrair ano de uma data: =Ano()</t>
+  </si>
+  <si>
+    <t>Extrair mês de uma data: =Mês()</t>
+  </si>
+  <si>
+    <t>Extrair dia de uma data: =Dia()</t>
+  </si>
+  <si>
+    <t>transformar dias em anos: =(HOJE()-G5)/365</t>
+  </si>
+  <si>
+    <t>Dias corridos</t>
+  </si>
+  <si>
+    <t>dias uteis</t>
   </si>
 </sst>
 </file>
@@ -316,20 +334,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -389,7 +394,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -472,7 +477,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -592,7 +597,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -673,7 +678,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -754,7 +759,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -832,7 +837,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -916,7 +921,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -997,7 +1002,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1117,7 +1122,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1200,7 +1205,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,7 +1286,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1364,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1438,7 +1443,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1520,7 +1525,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1608,7 +1613,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +1706,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1782,7 +1787,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1902,7 +1907,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1985,7 +1990,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2066,7 +2071,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2144,7 +2149,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2223,7 +2228,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2311,7 +2316,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2393,7 +2398,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2486,7 +2491,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2567,7 +2572,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2687,7 +2692,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2770,7 +2775,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2851,7 +2856,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2929,7 +2934,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3008,7 +3013,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3096,7 +3101,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3184,7 +3189,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3547,10 +3552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3643,7 +3648,7 @@
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="26">
         <f ca="1">NOW()</f>
-        <v>45348.726684259258</v>
+        <v>45348.740077314818</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
@@ -3657,9 +3662,25 @@
       <c r="O24" s="22"/>
     </row>
     <row r="25" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3791,8 +3812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3900,8 +3921,14 @@
       <c r="H5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
+      <c r="I5" s="16">
+        <f ca="1">(TODAY()-G5)/365</f>
+        <v>10.38082191780822</v>
+      </c>
+      <c r="J5" s="17">
+        <f>YEAR(G5)+5</f>
+        <v>2018</v>
+      </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -3916,7 +3943,10 @@
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11">
+        <f>YEAR(G5)</f>
+        <v>2013</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="12"/>
       <c r="I6" s="16"/>
@@ -3935,7 +3965,10 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="11">
+        <f>MONTH(G5)</f>
+        <v>10</v>
+      </c>
       <c r="G7" s="15"/>
       <c r="H7" s="12"/>
       <c r="I7" s="16"/>
@@ -3973,8 +4006,13 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="11">
+        <f>DAY(G5)</f>
+        <v>12</v>
+      </c>
+      <c r="G9" s="15">
+        <v>43544</v>
+      </c>
       <c r="H9" s="12"/>
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
@@ -3991,7 +4029,9 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="15">
+        <v>43554</v>
+      </c>
       <c r="H10" s="12"/>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
@@ -4007,8 +4047,13 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="27">
+        <f>G10-G9</f>
+        <v>10</v>
+      </c>
       <c r="H11" s="12"/>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
@@ -4024,8 +4069,13 @@
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="27">
+        <f>NETWORKDAYS(G9,G10)</f>
+        <v>8</v>
+      </c>
       <c r="H12" s="12"/>
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
@@ -5453,10 +5503,10 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <conditionalFormatting sqref="H5:H7">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>